<commit_message>
Excel aktarma ve pdf bitti
</commit_message>
<xml_diff>
--- a/typesofcells.xlsx
+++ b/typesofcells.xlsx
@@ -12,7 +12,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
+  <si>
+    <t xml:space="preserve">GÖZETİM MUAYENE VE EĞİTİM HİZMETLERİ  </t>
+  </si>
+  <si>
+    <t>MANYETİK  PARÇACIK MUAYENE RAPORU</t>
+  </si>
+  <si>
+    <t>MAGNETIC PARTICLE INSPECTİON REPORT</t>
+  </si>
   <si>
     <t>Müşteri
 Customer</t>
@@ -120,6 +129,9 @@
 Pole Distance</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>Muayene Bölgesi
 Examination Area</t>
   </si>
@@ -138,7 +150,7 @@
 Equipment</t>
   </si>
   <si>
-    <t>cihaz</t>
+    <t>evet</t>
   </si>
   <si>
     <t>Akım Tipi
@@ -157,7 +169,7 @@
 MP Carrier Medium</t>
   </si>
   <si>
-    <t>ortam</t>
+    <t>hayır</t>
   </si>
   <si>
     <t>Luxmetre/Işık Şiddeti
@@ -171,7 +183,7 @@
 Mag. Tech.</t>
   </si>
   <si>
-    <t>teknik</t>
+    <t>10</t>
   </si>
   <si>
     <t>Muayene Ortamı
@@ -192,7 +204,7 @@
 UV Light Intensity</t>
   </si>
   <si>
-    <t>şiddet</t>
+    <t>15</t>
   </si>
   <si>
     <t>Mıknatıs Giderimi
@@ -213,7 +225,7 @@
 Distance Of Light</t>
   </si>
   <si>
-    <t>fghfghfh</t>
+    <t>22</t>
   </si>
   <si>
     <t>Isıl İşlem
@@ -338,24 +350,15 @@
     <t>9</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>14</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
@@ -372,9 +375,6 @@
   </si>
   <si>
     <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
   </si>
   <si>
     <t>23</t>
@@ -434,15 +434,6 @@
   <si>
     <t>Adı Soyadı
 Name Surname</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>dfg</t>
-  </si>
-  <si>
-    <t>jhk</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -483,12 +474,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="6"/>
+        <fgColor indexed="45"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="6"/>
+        <fgColor indexed="45"/>
       </patternFill>
     </fill>
   </fills>
@@ -522,10 +513,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyBorder="true" applyFill="true">
       <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -538,13 +529,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>300683</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -576,13 +567,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>292086</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -615,7 +606,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -629,600 +620,664 @@
     <col min="10" max="10" width="12.00390625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" ht="40.0" customHeight="true">
-      <c r="A1" t="s" s="1">
+    <row r="1">
+      <c r="C1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+    </row>
+    <row r="2">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3">
+      <c r="C3" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="1">
+    </row>
+    <row r="4">
+      <c r="C4" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" ht="40.0" customHeight="true">
+      <c r="A5" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="G1" t="s" s="1">
+      <c r="B5" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="D5" t="s" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="1">
+      <c r="E5" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="G5" t="s" s="1">
         <v>7</v>
       </c>
-      <c r="D2" t="s" s="1">
+      <c r="H5" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="E2" t="s" s="2">
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="1">
         <v>9</v>
       </c>
-      <c r="G2" t="s" s="1">
+      <c r="B6" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="H2" t="s" s="2">
+      <c r="D6" t="s" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="1">
+      <c r="E6" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="G6" t="s" s="1">
         <v>13</v>
       </c>
-      <c r="D3" t="s" s="1">
+      <c r="H6" t="s" s="3">
         <v>14</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s" s="1">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="1">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s" s="1">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="G4" t="s" s="1">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="1">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="G5" t="s" s="1">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="3">
-        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="B7" t="s" s="3">
+        <v>16</v>
       </c>
       <c r="D7" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>31</v>
+        <v>17</v>
+      </c>
+      <c r="E7" t="s" s="3">
+        <v>18</v>
       </c>
       <c r="G7" t="s" s="1">
-        <v>32</v>
-      </c>
-      <c r="H7" t="s" s="2">
-        <v>33</v>
+        <v>19</v>
+      </c>
+      <c r="H7" t="s" s="3">
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>35</v>
+        <v>21</v>
+      </c>
+      <c r="B8" t="s" s="3">
+        <v>22</v>
       </c>
       <c r="D8" t="s" s="1">
-        <v>36</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="E8" s="3"/>
       <c r="G8" t="s" s="1">
-        <v>37</v>
-      </c>
-      <c r="H8" t="s" s="2">
-        <v>38</v>
+        <v>24</v>
+      </c>
+      <c r="H8" t="s" s="3">
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
-        <v>39</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>40</v>
+        <v>26</v>
+      </c>
+      <c r="B9" t="s" s="3">
+        <v>27</v>
       </c>
       <c r="D9" t="s" s="1">
-        <v>41</v>
-      </c>
-      <c r="E9" t="s" s="2">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="G9" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="1">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D10" t="s" s="1">
-        <v>45</v>
-      </c>
-      <c r="E10" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="G10" t="s" s="1">
-        <v>47</v>
-      </c>
-      <c r="H10" t="s" s="2">
-        <v>48</v>
-      </c>
+      <c r="A10" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
-        <v>49</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>50</v>
+        <v>32</v>
+      </c>
+      <c r="B11" t="s" s="3">
+        <v>33</v>
       </c>
       <c r="D11" t="s" s="1">
-        <v>51</v>
-      </c>
-      <c r="E11" t="s" s="2">
-        <v>52</v>
+        <v>34</v>
+      </c>
+      <c r="E11" t="s" s="3">
+        <v>35</v>
       </c>
       <c r="G11" t="s" s="1">
-        <v>53</v>
-      </c>
-      <c r="H11" t="s" s="2">
-        <v>54</v>
+        <v>36</v>
+      </c>
+      <c r="H11" t="s" s="3">
+        <v>37</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s" s="3">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="G12" t="s" s="1">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="1">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s" s="3">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s" s="1">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s" s="3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="1">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s" s="3">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s" s="1">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s" s="3">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s" s="1">
+        <v>51</v>
+      </c>
+      <c r="H14" t="s" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="1">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s" s="3">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s" s="1">
         <v>55</v>
       </c>
-      <c r="B12" t="s" s="2">
+      <c r="E15" t="s" s="3">
         <v>56</v>
       </c>
-      <c r="D12" t="s" s="1">
+      <c r="G15" t="s" s="1">
         <v>57</v>
       </c>
-      <c r="E12" t="s" s="2">
+      <c r="H15" t="s" s="3">
         <v>58</v>
       </c>
-      <c r="G12" t="s" s="1">
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="1">
         <v>59</v>
       </c>
-      <c r="H12" t="s" s="2">
+      <c r="B16" t="s" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="G13" t="s" s="1">
+      <c r="D16" t="s" s="1">
         <v>61</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="G14" t="s" s="1">
+      <c r="E16" t="s" s="3">
         <v>62</v>
       </c>
-      <c r="H14" t="s" s="1">
+      <c r="G16" t="s" s="1">
         <v>63</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="G15" t="s" s="1">
+      <c r="H16" t="s" s="3">
         <v>64</v>
-      </c>
-      <c r="H15" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="G16" t="s" s="1">
-        <v>66</v>
-      </c>
-      <c r="H16" t="s" s="1">
-        <v>67</v>
       </c>
     </row>
     <row r="17">
       <c r="G17" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18">
+      <c r="G18" t="s" s="1">
+        <v>66</v>
+      </c>
+      <c r="H18" t="s" s="1">
+        <v>67</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19">
+      <c r="G19" t="s" s="1">
         <v>68</v>
       </c>
-      <c r="H17" t="s" s="1">
+      <c r="H19" t="s" s="1">
         <v>69</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="1">
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20">
+      <c r="G20" t="s" s="1">
         <v>70</v>
       </c>
-      <c r="B19" t="s" s="2">
+      <c r="H20" t="s" s="1">
         <v>71</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="1">
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21">
+      <c r="G21" t="s" s="1">
         <v>72</v>
       </c>
-      <c r="B20" t="s" s="2">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="1">
+      <c r="H21" t="s" s="1">
         <v>73</v>
       </c>
-      <c r="B21" t="s" s="2">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="3">
-        <v>75</v>
-      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="1">
         <v>76</v>
       </c>
-      <c r="B23" t="s" s="1">
+      <c r="B24" t="s" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="1">
         <v>77</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" t="s" s="1">
+      <c r="B25" t="s" s="3">
         <v>78</v>
       </c>
-      <c r="E23" t="s" s="1">
-        <v>79</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" t="s" s="1">
-        <v>80</v>
-      </c>
-      <c r="H23" t="s" s="1">
-        <v>81</v>
-      </c>
-      <c r="I23" t="s" s="1">
-        <v>82</v>
-      </c>
-      <c r="J23" t="s" s="1">
-        <v>83</v>
-      </c>
-      <c r="K23" t="s" s="1">
-        <v>84</v>
-      </c>
-      <c r="L23" s="1"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="E24" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="G24" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H24" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="I24" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="J24" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="B25" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="D25" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="E25" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="G25" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="H25" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="I25" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="J25" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="K25" s="2"/>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="1">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" t="s" s="1">
+        <v>82</v>
+      </c>
+      <c r="E27" t="s" s="1">
+        <v>83</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" t="s" s="1">
+        <v>84</v>
+      </c>
+      <c r="H27" t="s" s="1">
+        <v>85</v>
+      </c>
+      <c r="I27" t="s" s="1">
         <v>86</v>
       </c>
-      <c r="B26" t="s" s="2">
+      <c r="J27" t="s" s="1">
+        <v>87</v>
+      </c>
+      <c r="K27" t="s" s="1">
+        <v>88</v>
+      </c>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s" s="3">
+        <v>89</v>
+      </c>
+      <c r="E28" t="s" s="3">
+        <v>90</v>
+      </c>
+      <c r="G28" t="s" s="3">
+        <v>91</v>
+      </c>
+      <c r="H28" t="s" s="3">
+        <v>92</v>
+      </c>
+      <c r="I28" t="s" s="3">
+        <v>93</v>
+      </c>
+      <c r="J28" t="s" s="3">
+        <v>94</v>
+      </c>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="3">
+        <v>89</v>
+      </c>
+      <c r="B29" t="s" s="3">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s" s="3">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s" s="3">
+        <v>48</v>
+      </c>
+      <c r="G29" t="s" s="3">
+        <v>97</v>
+      </c>
+      <c r="H29" t="s" s="3">
         <v>98</v>
       </c>
-      <c r="D26" t="s" s="2">
+      <c r="I29" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="J29" t="s" s="3">
         <v>99</v>
       </c>
-      <c r="E26" t="s" s="2">
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="3">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s" s="3">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s" s="3">
         <v>100</v>
       </c>
-      <c r="G26" t="s" s="2">
+      <c r="E30" t="s" s="3">
         <v>101</v>
       </c>
-      <c r="H26" t="s" s="2">
+      <c r="G30" t="s" s="3">
         <v>102</v>
       </c>
-      <c r="I26" t="s" s="2">
+      <c r="H30" t="s" s="3">
         <v>103</v>
       </c>
-      <c r="J26" t="s" s="2">
+      <c r="I30" t="s" s="3">
         <v>104</v>
       </c>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="B27" t="s" s="2">
+      <c r="J30" t="s" s="3">
         <v>105</v>
       </c>
-      <c r="D27" t="s" s="2">
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="3">
+        <v>91</v>
+      </c>
+      <c r="B31" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s" s="3">
         <v>106</v>
       </c>
-      <c r="E27" t="s" s="2">
+      <c r="E31" t="s" s="3">
         <v>107</v>
       </c>
-      <c r="G27" t="s" s="2">
+      <c r="G31" t="s" s="3">
         <v>108</v>
       </c>
-      <c r="H27" t="s" s="2">
+      <c r="H31" t="s" s="3">
         <v>109</v>
       </c>
-      <c r="I27" t="s" s="2">
+      <c r="I31" t="s" s="3">
         <v>110</v>
       </c>
-      <c r="J27" t="s" s="2">
+      <c r="J31" t="s" s="3">
         <v>111</v>
       </c>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="B28" t="s" s="2">
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="3">
+        <v>92</v>
+      </c>
+      <c r="B32" t="s" s="3">
         <v>112</v>
       </c>
-      <c r="D28" t="s" s="2">
+      <c r="D32" t="s" s="3">
         <v>113</v>
       </c>
-      <c r="E28" t="s" s="2">
+      <c r="E32" t="s" s="3">
         <v>114</v>
       </c>
-      <c r="G28" t="s" s="2">
+      <c r="G32" t="s" s="3">
         <v>115</v>
       </c>
-      <c r="H28" t="s" s="2">
+      <c r="H32" t="s" s="3">
         <v>116</v>
       </c>
-      <c r="I28" t="s" s="2">
+      <c r="I32" t="s" s="3">
         <v>117</v>
       </c>
-      <c r="J28" t="s" s="2">
+      <c r="J32" t="s" s="3">
         <v>118</v>
       </c>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="1">
-        <v>119</v>
-      </c>
-      <c r="B29" t="s" s="1">
-        <v>120</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" t="s" s="1">
-        <v>121</v>
-      </c>
-      <c r="E29" t="s" s="1">
-        <v>122</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" t="s" s="1">
-        <v>123</v>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="1">
-        <v>124</v>
-      </c>
-      <c r="B30" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="D30" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="E30" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="G30" t="s" s="2">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s" s="1">
-        <v>129</v>
-      </c>
-      <c r="B31" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="D31" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="E31" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="G31" t="s" s="2">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="1">
-        <v>130</v>
-      </c>
-      <c r="B32" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="D32" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="E32" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="G32" t="s" s="2">
-        <v>128</v>
-      </c>
+      <c r="K32" s="3"/>
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
-        <v>131</v>
-      </c>
-      <c r="B33" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="B33" t="s" s="1">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" t="s" s="1">
+        <v>121</v>
+      </c>
+      <c r="E33" t="s" s="1">
+        <v>122</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" t="s" s="1">
+        <v>123</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="1">
+        <v>124</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="G34" t="s" s="3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="1">
+        <v>126</v>
+      </c>
+      <c r="B35" t="s" s="3">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s" s="3">
+        <v>78</v>
+      </c>
+      <c r="E35" t="s" s="3">
+        <v>78</v>
+      </c>
+      <c r="G35" t="s" s="3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="1">
+        <v>127</v>
+      </c>
+      <c r="B36" t="s" s="3">
+        <v>78</v>
+      </c>
+      <c r="D36" t="s" s="3">
+        <v>78</v>
+      </c>
+      <c r="E36" t="s" s="3">
+        <v>78</v>
+      </c>
+      <c r="G36" t="s" s="3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="1">
         <v>128</v>
       </c>
-      <c r="D33" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="E33" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="G33" t="s" s="2">
-        <v>128</v>
+      <c r="B37" t="s" s="3">
+        <v>125</v>
+      </c>
+      <c r="D37" t="s" s="3">
+        <v>125</v>
+      </c>
+      <c r="E37" t="s" s="3">
+        <v>125</v>
+      </c>
+      <c r="G37" t="s" s="3">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="75">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+  <mergeCells count="78">
+    <mergeCell ref="C1:L2"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="C4:L4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="H6:L6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H7:L7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="H8:I9"/>
+    <mergeCell ref="H8:L8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="A10:L10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H11:L11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H12:L13"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="H15:L15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="G17:L17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="B25:L25"/>
+    <mergeCell ref="A26:L26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="K27:L27"/>
@@ -1231,19 +1286,31 @@
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:L29"/>
+    <mergeCell ref="K29:L29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:L30"/>
+    <mergeCell ref="K30:L30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:L31"/>
+    <mergeCell ref="K31:L31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:L32"/>
+    <mergeCell ref="K32:L32"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="G33:L33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:L34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:L35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:L36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:L37"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
son bir iki küçük detay kaldı onun dışında her şey okey
</commit_message>
<xml_diff>
--- a/typesofcells.xlsx
+++ b/typesofcells.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="132">
   <si>
     <t xml:space="preserve">GÖZETİM MUAYENE VE EĞİTİM HİZMETLERİ  </t>
   </si>
@@ -27,7 +27,7 @@
 Customer</t>
   </si>
   <si>
-    <t>egeuzma</t>
+    <t>ege</t>
   </si>
   <si>
     <t>Muayene Prosedürü
@@ -69,7 +69,7 @@
 Inspection Place</t>
   </si>
   <si>
-    <t>ankara</t>
+    <t>istanbul</t>
   </si>
   <si>
     <t>Resim No
@@ -434,6 +434,15 @@
   <si>
     <t>Adı Soyadı
 Name Surname</t>
+  </si>
+  <si>
+    <t>Ege</t>
+  </si>
+  <si>
+    <t>Barış</t>
+  </si>
+  <si>
+    <t>Serra</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -1173,33 +1182,39 @@
       <c r="A34" t="s" s="1">
         <v>124</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="B34" t="s" s="3">
+        <v>125</v>
+      </c>
+      <c r="D34" t="s" s="3">
+        <v>126</v>
+      </c>
+      <c r="E34" t="s" s="3">
+        <v>127</v>
+      </c>
       <c r="G34" t="s" s="3">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="1">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B35" t="s" s="3">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D35" t="s" s="3">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="E35" t="s" s="3">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G35" t="s" s="3">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="1">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B36" t="s" s="3">
         <v>78</v>
@@ -1211,24 +1226,24 @@
         <v>78</v>
       </c>
       <c r="G36" t="s" s="3">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="1">
+        <v>131</v>
+      </c>
+      <c r="B37" t="s" s="3">
         <v>128</v>
       </c>
-      <c r="B37" t="s" s="3">
-        <v>125</v>
-      </c>
       <c r="D37" t="s" s="3">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E37" t="s" s="3">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G37" t="s" s="3">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>